<commit_message>
push attempt at regex for getting network info, I hate regex
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -52,10 +52,10 @@
     <t xml:space="preserve">comments</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.1.145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">laptop</t>
+    <t xml:space="preserve">192.168.1.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">server</t>
   </si>
   <si>
     <t xml:space="preserve">compute</t>
@@ -64,10 +64,10 @@
     <t xml:space="preserve">zeus</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.1.147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">camera</t>
+    <t xml:space="preserve">192.168.1.241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuum</t>
   </si>
   <si>
     <t xml:space="preserve">pit_reader</t>
@@ -76,19 +76,19 @@
     <t xml:space="preserve">lmc</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.1.1</t>
+    <t xml:space="preserve">192.168.1.249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.1.254</t>
   </si>
   <si>
     <t xml:space="preserve">gateway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.1.215</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
   </si>
   <si>
     <t xml:space="preserve">mmcu</t>
@@ -225,10 +225,10 @@
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.57"/>

</xml_diff>

<commit_message>
postgres append now functional
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t xml:space="preserve">ip_address</t>
   </si>
@@ -52,10 +52,10 @@
     <t xml:space="preserve">comments</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.44.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">server</t>
+    <t xml:space="preserve">192.168.86.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gateway</t>
   </si>
   <si>
     <t xml:space="preserve">compute</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">zeus</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.44.25</t>
+    <t xml:space="preserve">192.168.86.40</t>
   </si>
   <si>
     <t xml:space="preserve">vacuum</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">lmc</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.44.155</t>
+    <t xml:space="preserve">192.168.86.46</t>
   </si>
   <si>
     <t xml:space="preserve">tv</t>
@@ -85,19 +85,16 @@
     <t xml:space="preserve">mmcd</t>
   </si>
   <si>
-    <t xml:space="preserve">10.30.8.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gateway</t>
+    <t xml:space="preserve">192.168.86.195</t>
   </si>
   <si>
     <t xml:space="preserve">mmcu</t>
   </si>
   <si>
-    <t xml:space="preserve">192.168.1.64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.1.254</t>
+    <t xml:space="preserve">10.10.50.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
   </si>
 </sst>
 </file>
@@ -219,10 +216,10 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.57"/>
@@ -234,7 +231,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="75.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="11" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="11" style="0" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,7 +284,7 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
@@ -307,7 +304,7 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
@@ -327,7 +324,7 @@
         <v>-119.0558</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
@@ -347,18 +344,18 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>41</v>
@@ -367,40 +364,21 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="1" t="n">
-        <v>41.99999</v>
+        <v>11.54356</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>-117.87666</v>
+        <v>45.79404</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>41.99999</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>-117.87666</v>
-      </c>
-    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>